<commit_message>
Project updated by lavanya
</commit_message>
<xml_diff>
--- a/src/test/resources/AddressData.xlsx
+++ b/src/test/resources/AddressData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alakshmanan\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EDF2AAE-AA80-4408-BBA8-D7239CA1C9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C469E6EB-5CC8-4660-9563-5D44C40CBB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="1845" windowWidth="12930" windowHeight="11385" xr2:uid="{365CA22A-97D7-4B96-8BDA-F3B182BCE418}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{365CA22A-97D7-4B96-8BDA-F3B182BCE418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,19 +52,19 @@
     <t>City</t>
   </si>
   <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>TamilNadu</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
     <t>Angitha</t>
   </si>
   <si>
-    <t>11,Mepzs</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>TamilNadu</t>
-  </si>
-  <si>
-    <t>India</t>
+    <t>Mepz</t>
   </si>
 </sst>
 </file>
@@ -423,7 +419,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,22 +454,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>600045</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -674,9 +670,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{248D98E3-90D0-4C77-B2A1-7ECC7B76CB1D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{248D98E3-90D0-4C77-B2A1-7ECC7B76CB1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7edc6231-c27a-4153-ba33-96fd73dccd28"/>
+    <ds:schemaRef ds:uri="ef295c0c-43be-4c7d-8076-bfd0f9603fc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B21220D2-E53A-46B6-A269-1DD52981B2E0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B21220D2-E53A-46B6-A269-1DD52981B2E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>